<commit_message>
Added option to print to excel file
</commit_message>
<xml_diff>
--- a/prediction.xlsx
+++ b/prediction.xlsx
@@ -493,20 +493,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1254544705152512</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01167208142578602</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.001049823244102299</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.861823558807373</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -521,16 +521,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6899406909942627</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0002454060304444283</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.000127273757243529</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3096867203712463</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -545,16 +545,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9996182918548584</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>3.287518666184042e-07</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0003530006215441972</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2.844139089575037e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -569,16 +569,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9987255930900574</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1.042131430040172e-06</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.001188269350677729</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>8.499823161400855e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9997125267982483</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>4.873547823081026e-07</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.000185364595381543</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0001016375972540118</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -617,16 +617,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9078434705734253</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0007434803992509842</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.002896340563893318</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.08851666748523712</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -641,16 +641,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9825069308280945</v>
+        <v>0.3386495073309164</v>
       </c>
       <c r="D8" t="n">
-        <v>2.142191988241393e-05</v>
+        <v>0.3306152359259172</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0172146949917078</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0002570018987171352</v>
+        <v>0.3307352567431665</v>
       </c>
     </row>
     <row r="9">
@@ -665,16 +665,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9966049194335938</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>8.386825356865302e-06</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.003078254871070385</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0003084396303165704</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -685,20 +685,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.9992682337760925</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>2.43569775193464e-06</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0002807224809657782</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0004485311801545322</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -713,16 +713,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.9993313550949097</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>5.148715445102425e-07</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0006072833784855902</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>6.078135629650205e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -737,16 +737,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9987701773643494</v>
+        <v>0.6653830943429145</v>
       </c>
       <c r="D12" t="n">
-        <v>4.853695827478077e-07</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.001193903852254152</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>3.534495044732466e-05</v>
+        <v>0.3346169056570855</v>
       </c>
     </row>
     <row r="13">
@@ -757,20 +757,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.9998304843902588</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>9.537885858890149e-08</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>9.860544378170744e-05</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>7.07686849636957e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -781,20 +781,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.9965569972991943</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>6.62167167320149e-06</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.003081200877204537</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>0.000355272670276463</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -805,20 +805,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.9992719292640686</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>5.66267772228457e-07</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0006684098043479025</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>5.909619358135387e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -829,20 +829,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.9989859461784363</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>4.68422854282835e-07</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0009944617049768567</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>1.909516504383646e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -853,20 +853,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.9998648166656494</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>7.021497339110283e-08</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>9.506788774160668e-05</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>4.000402623205446e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -877,20 +877,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.9996250867843628</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>6.860036023681459e-07</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0002582302549853921</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0001160189276561141</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -901,20 +901,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.9991933703422546</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>3.126221201910084e-07</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0007910442072898149</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>1.523479386378312e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -929,16 +929,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.9982965588569641</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>2.04431967176788e-06</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0001467889233026654</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.001554723596200347</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -949,20 +949,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.9992216825485229</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>1.48426238411048e-06</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0006129523389972746</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.000163879114552401</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -977,16 +977,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.8474880456924438</v>
+        <v>0.6685935153207773</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0006711880560033023</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.1499811410903931</v>
+        <v>0.3314064846792227</v>
       </c>
       <c r="F22" t="n">
-        <v>0.00185960263479501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -997,20 +997,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.9896776676177979</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>2.515440655770362e-06</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0.01030165329575539</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>1.809004425012972e-05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.9994619488716125</v>
+        <v>0.6671008803626376</v>
       </c>
       <c r="D24" t="n">
-        <v>3.020144276888459e-07</v>
+        <v>0.3328991196373624</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0004894697340205312</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>4.828548480872996e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1049,16 +1049,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.9987605810165405</v>
+        <v>0.671362379512858</v>
       </c>
       <c r="D25" t="n">
-        <v>4.065715017986804e-07</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0.001214519841596484</v>
+        <v>0.3286376204871418</v>
       </c>
       <c r="F25" t="n">
-        <v>2.446774487907533e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1073,16 +1073,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.9997400641441345</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>4.201281811333502e-08</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0.0002519504050724208</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>7.990238373167813e-06</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>